<commit_message>
Add _Sidebar, remove Getting-Started.
</commit_message>
<xml_diff>
--- a/05_wiki_changelog/wiki-changelog.xlsx
+++ b/05_wiki_changelog/wiki-changelog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>Reordered links in Getting Started.</t>
+  </si>
+  <si>
+    <t>Getting-Started</t>
+  </si>
+  <si>
+    <t>Removed from sidebar; duplicated sidebar links.</t>
+  </si>
+  <si>
+    <t>Installing-FFmpeg</t>
   </si>
 </sst>
 </file>
@@ -429,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,13 +479,13 @@
         <v>42104</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -484,32 +493,32 @@
         <v>42104</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>42103</v>
+        <v>42104</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>42103</v>
+        <v>42104</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>4</v>
@@ -518,63 +527,63 @@
         <v>15</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>42104</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>42103</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>42103</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>42103</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>42092</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>42092</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>42092</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -582,26 +591,68 @@
         <v>42092</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
+        <v>42092</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42092</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42092</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>42090</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>